<commit_message>
bare bones spec misc_id
</commit_message>
<xml_diff>
--- a/meta/unc_vernacular.xlsx
+++ b/meta/unc_vernacular.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10185"/>
   </bookViews>
   <sheets>
     <sheet name="blocks" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,8 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId6"/>
-    <pivotCache cacheId="15" r:id="rId7"/>
+    <pivotCache cacheId="22" r:id="rId6"/>
+    <pivotCache cacheId="23" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1026,67 +1026,6 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1134,6 +1073,67 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4790,7 +4790,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="nvfieldsummary" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="nvfieldsummary" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -4869,7 +4869,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="vfieldsummary" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="vfieldsummary" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B59" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -5131,20 +5131,20 @@
   <tableColumns count="10">
     <tableColumn id="1" name="Language"/>
     <tableColumn id="2" name="Block"/>
-    <tableColumn id="5" name="codepoint_range" dataDxfId="3">
+    <tableColumn id="5" name="codepoint_range" dataDxfId="10">
       <calculatedColumnFormula>IF(blocks[codepoints_override]=".","[\x"&amp;D2&amp;"-\x"&amp;E2&amp;"]",blocks[codepoints_override])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="codepoint_begin" dataDxfId="6"/>
+    <tableColumn id="3" name="codepoint_begin" dataDxfId="9"/>
     <tableColumn id="4" name="codepoint_end"/>
     <tableColumn id="8" name="880s_checked"/>
-    <tableColumn id="11" name="non880s_checked" dataDxfId="1"/>
-    <tableColumn id="9" name="Total_880s" dataDxfId="5">
+    <tableColumn id="11" name="non880s_checked" dataDxfId="8"/>
+    <tableColumn id="9" name="Total_880s" dataDxfId="7">
       <calculatedColumnFormula>GETPIVOTDATA("880",vfield_summary,"Block",blocks[Block])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Total_non880" dataDxfId="0">
+    <tableColumn id="12" name="Total_non880" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(blocks[non880s_checked]),"",GETPIVOTDATA("Field_count",nvfield_summary!$A$3,"Block",blocks[Block]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="codepoints_override" dataDxfId="4"/>
+    <tableColumn id="10" name="codepoints_override" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5154,7 +5154,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C160" totalsRowShown="0">
   <autoFilter ref="A1:C160"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Block" dataDxfId="2"/>
+    <tableColumn id="1" name="Block" dataDxfId="4"/>
     <tableColumn id="2" name="Field"/>
     <tableColumn id="3" name="Field_count"/>
   </tableColumns>
@@ -5163,12 +5163,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="vfields" displayName="vfields" ref="A1:C545" totalsRowShown="0" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="vfields" displayName="vfields" ref="A1:C545" totalsRowShown="0" dataDxfId="3">
   <autoFilter ref="A1:C545"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Block" dataDxfId="10"/>
-    <tableColumn id="2" name="Field" dataDxfId="9"/>
-    <tableColumn id="4" name="880" dataDxfId="8"/>
+    <tableColumn id="1" name="Block" dataDxfId="2"/>
+    <tableColumn id="2" name="Field" dataDxfId="1"/>
+    <tableColumn id="4" name="880" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5440,7 +5440,7 @@
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
supporting docs for linking fields, included work
</commit_message>
<xml_diff>
--- a/meta/unc_vernacular.xlsx
+++ b/meta/unc_vernacular.xlsx
@@ -20,8 +20,8 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="22" r:id="rId6"/>
-    <pivotCache cacheId="23" r:id="rId7"/>
+    <pivotCache cacheId="103" r:id="rId6"/>
+    <pivotCache cacheId="104" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -940,6 +940,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -4790,7 +4791,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="nvfieldsummary" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="nvfieldsummary" cacheId="104" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -4869,7 +4870,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="vfieldsummary" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="vfieldsummary" cacheId="103" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B59" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -5440,7 +5441,7 @@
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7367,8 +7368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C160"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C153" sqref="C153"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9271,8 +9272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C545"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>